<commit_message>
Screenshots after models done
</commit_message>
<xml_diff>
--- a/train_networks/comparison.xlsx
+++ b/train_networks/comparison.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester2\Images\Project\egh444-group-project\train_networks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E0FC49-FA16-43B3-A5A8-95561F91F4C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A9F86C-D1D7-40BC-9EE0-3E39A2E43D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="9200" windowWidth="13580" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4850" yWindow="2900" windowWidth="12740" windowHeight="7250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>ResNet-18</t>
   </si>
@@ -33,9 +42,6 @@
     <t>AlexNet</t>
   </si>
   <si>
-    <t>MobileNet</t>
-  </si>
-  <si>
     <t>Validation</t>
   </si>
   <si>
@@ -54,16 +60,52 @@
     <t>Size</t>
   </si>
   <si>
-    <t>640MB</t>
-  </si>
-  <si>
-    <t>250MB</t>
-  </si>
-  <si>
-    <t>120MB</t>
-  </si>
-  <si>
-    <t>30MB</t>
+    <t>VGG-16</t>
+  </si>
+  <si>
+    <t>MobileNetV2</t>
+  </si>
+  <si>
+    <t>61M</t>
+  </si>
+  <si>
+    <t>11M</t>
+  </si>
+  <si>
+    <t>138M</t>
+  </si>
+  <si>
+    <t>24M</t>
+  </si>
+  <si>
+    <t>3.4M</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>Measure size as net only not entire workspace</t>
+  </si>
+  <si>
+    <t>6 Epochs</t>
+  </si>
+  <si>
+    <t>1 Epoch</t>
+  </si>
+  <si>
+    <t>8MB</t>
+  </si>
+  <si>
+    <t>200MB</t>
+  </si>
+  <si>
+    <t>80MB</t>
+  </si>
+  <si>
+    <t>40MB</t>
+  </si>
+  <si>
+    <t>500MB</t>
   </si>
 </sst>
 </file>
@@ -87,18 +129,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -114,12 +150,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -190,8 +244,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -199,49 +257,68 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,132 +601,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="6" width="10.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.08984375" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="17" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="24"/>
+      <c r="B1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="25"/>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.87780000000000002</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.9284</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.94</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.9667</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0.95020000000000004</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.9778</v>
+      </c>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.89839999999999998</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.91110000000000002</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.92969999999999997</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.9778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.9556</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.93930000000000002</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.9556</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.96789999999999998</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.9778</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.91879999999999995</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.91110000000000002</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.92969999999999997</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.93520000000000003</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.9667</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.95909999999999995</v>
+      </c>
+      <c r="K6" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10">
+        <v>0.97340000000000004</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.9778</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.9284</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.92220000000000002</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0.94</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.9667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.91539999999999999</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.93330000000000002</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0.92969999999999997</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.93330000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.92220000000000002</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.9556</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.93930000000000002</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.9556</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.92969999999999997</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.94440000000000002</v>
-      </c>
-      <c r="E6" s="16">
-        <v>0.93520000000000003</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.9667</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="17" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
+  <mergeCells count="5">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
confusions, comparison spreadsheet filled out
</commit_message>
<xml_diff>
--- a/train_networks/comparison.xlsx
+++ b/train_networks/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester2\Images\Project\egh444-group-project\train_networks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A9F86C-D1D7-40BC-9EE0-3E39A2E43D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CB8A6F-6DD5-427E-9134-E933E658637F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4850" yWindow="2900" windowWidth="12740" windowHeight="7250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19170" yWindow="4400" windowWidth="14770" windowHeight="7250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>ResNet-18</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>Test Set</t>
-  </si>
-  <si>
     <t>3 Epochs</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Params</t>
   </si>
   <si>
-    <t>Measure size as net only not entire workspace</t>
-  </si>
-  <si>
     <t>6 Epochs</t>
   </si>
   <si>
@@ -106,13 +100,29 @@
   </si>
   <si>
     <t>500MB</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>90 images</t>
+  </si>
+  <si>
+    <t>133 images</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +138,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +189,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -280,11 +303,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,7 +350,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -321,8 +362,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,73 +674,80 @@
     <col min="3" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="10.08984375" customWidth="1"/>
     <col min="10" max="10" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="26" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="23"/>
+      <c r="B1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="27"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="31"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="25"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="24"/>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
+      <c r="E2" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
+      <c r="G2" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>3</v>
+      <c r="I2" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="K2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="28"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11">
         <v>0.87239999999999995</v>
@@ -700,23 +767,27 @@
       <c r="I3" s="12">
         <v>0.9667</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="35">
         <v>0.95020000000000004</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="18">
         <v>0.9778</v>
       </c>
-      <c r="L3" s="18"/>
+      <c r="L3" s="34">
+        <v>0.84209999999999996</v>
+      </c>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>11</v>
+      <c r="B4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="11">
         <v>0.89839999999999998</v>
@@ -739,19 +810,23 @@
       <c r="J4" s="11">
         <v>0.96250000000000002</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="18">
         <v>0.9778</v>
       </c>
+      <c r="L4" s="36">
+        <v>0.92479999999999996</v>
+      </c>
+      <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="11">
         <v>0.89500000000000002</v>
@@ -771,22 +846,26 @@
       <c r="I5" s="12">
         <v>0.9556</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="37">
         <v>0.96789999999999998</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="18">
         <v>0.9778</v>
       </c>
+      <c r="L5" s="36">
+        <v>0.93230000000000002</v>
+      </c>
+      <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="11">
         <v>0.91879999999999995</v>
@@ -809,36 +888,72 @@
       <c r="J6" s="11">
         <v>0.95909999999999995</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="29">
         <v>1</v>
       </c>
+      <c r="L6" s="36">
+        <v>0.92479999999999996</v>
+      </c>
+      <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="10">
+      <c r="H7" s="38">
         <v>0.97340000000000004</v>
       </c>
       <c r="I7" s="13">
         <v>0.9778</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="30"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="17" t="s">
-        <v>16</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="33">
+        <v>30</v>
+      </c>
+      <c r="G9" s="33">
+        <v>30</v>
+      </c>
+      <c r="H9" s="33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>45</v>
+      </c>
+      <c r="H10">
+        <f>133-45-45</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +961,7 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>